<commit_message>
fix: spelling in orderform
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.34.mip_no_delivery.xlsx
+++ b/tests/fixtures/orderforms/1508.34.mip_no_delivery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Documents/clinicalGenomics/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EFFC47-630F-014F-A073-79DB643F81C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2EC1F4-B6DE-F845-B051-7A27EE0FA44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="840">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -3604,9 +3604,6 @@
   </si>
   <si>
     <t>comment</t>
-  </si>
-  <si>
-    <t>Inhertired cancer</t>
   </si>
 </sst>
 </file>
@@ -5850,8 +5847,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -13554,7 +13551,7 @@
         <v>71</v>
       </c>
       <c r="U15" s="87" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V15" s="101" t="s">
         <v>70</v>
@@ -14635,7 +14632,7 @@
         <v>71</v>
       </c>
       <c r="U16" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V16" s="160" t="s">
         <v>80</v>
@@ -15700,7 +15697,7 @@
         <v>71</v>
       </c>
       <c r="U17" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V17" s="160" t="s">
         <v>80</v>
@@ -16761,7 +16758,7 @@
         <v>71</v>
       </c>
       <c r="U18" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V18" s="160" t="s">
         <v>70</v>
@@ -17822,7 +17819,7 @@
         <v>71</v>
       </c>
       <c r="U19" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V19" s="160" t="s">
         <v>70</v>
@@ -18883,7 +18880,7 @@
         <v>71</v>
       </c>
       <c r="U20" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V20" s="160" t="s">
         <v>70</v>
@@ -19944,7 +19941,7 @@
         <v>71</v>
       </c>
       <c r="U21" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V21" s="160" t="s">
         <v>70</v>
@@ -21005,7 +21002,7 @@
         <v>71</v>
       </c>
       <c r="U22" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V22" s="160" t="s">
         <v>70</v>
@@ -22066,7 +22063,7 @@
         <v>71</v>
       </c>
       <c r="U23" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V23" s="160" t="s">
         <v>70</v>
@@ -23127,7 +23124,7 @@
         <v>71</v>
       </c>
       <c r="U24" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V24" s="160" t="s">
         <v>70</v>
@@ -24188,7 +24185,7 @@
         <v>71</v>
       </c>
       <c r="U25" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V25" s="160" t="s">
         <v>70</v>
@@ -25249,7 +25246,7 @@
         <v>71</v>
       </c>
       <c r="U26" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V26" s="160" t="s">
         <v>70</v>
@@ -26311,7 +26308,7 @@
       </c>
       <c r="T27"/>
       <c r="U27" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V27" s="160" t="s">
         <v>70</v>
@@ -26382,7 +26379,7 @@
         <v>71</v>
       </c>
       <c r="U28" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V28" s="160" t="s">
         <v>70</v>
@@ -27443,7 +27440,7 @@
         <v>71</v>
       </c>
       <c r="U29" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V29" s="160" t="s">
         <v>70</v>
@@ -28504,7 +28501,7 @@
         <v>71</v>
       </c>
       <c r="U30" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V30" s="160" t="s">
         <v>70</v>
@@ -29565,7 +29562,7 @@
         <v>71</v>
       </c>
       <c r="U31" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V31" s="160" t="s">
         <v>70</v>
@@ -30626,7 +30623,7 @@
         <v>71</v>
       </c>
       <c r="U32" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V32" s="160" t="s">
         <v>70</v>
@@ -31687,7 +31684,7 @@
         <v>71</v>
       </c>
       <c r="U33" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V33" s="160" t="s">
         <v>70</v>
@@ -32748,7 +32745,7 @@
         <v>71</v>
       </c>
       <c r="U34" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V34" s="160" t="s">
         <v>70</v>
@@ -33809,7 +33806,7 @@
         <v>71</v>
       </c>
       <c r="U35" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V35" s="160" t="s">
         <v>70</v>
@@ -34871,7 +34868,7 @@
       </c>
       <c r="T36"/>
       <c r="U36" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V36" s="160" t="s">
         <v>70</v>
@@ -34943,7 +34940,7 @@
       </c>
       <c r="T37"/>
       <c r="U37" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V37" s="160" t="s">
         <v>70</v>
@@ -35015,7 +35012,7 @@
       </c>
       <c r="T38"/>
       <c r="U38" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V38" s="160" t="s">
         <v>70</v>
@@ -35086,7 +35083,7 @@
         <v>81</v>
       </c>
       <c r="U39" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V39" s="160" t="s">
         <v>70</v>
@@ -36147,7 +36144,7 @@
         <v>81</v>
       </c>
       <c r="U40" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V40" s="160" t="s">
         <v>70</v>
@@ -37208,7 +37205,7 @@
         <v>81</v>
       </c>
       <c r="U41" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V41" s="160" t="s">
         <v>70</v>
@@ -38269,7 +38266,7 @@
         <v>81</v>
       </c>
       <c r="U42" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V42" s="160" t="s">
         <v>70</v>
@@ -39330,7 +39327,7 @@
         <v>81</v>
       </c>
       <c r="U43" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V43" s="160" t="s">
         <v>70</v>
@@ -40391,7 +40388,7 @@
         <v>81</v>
       </c>
       <c r="U44" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V44" s="160" t="s">
         <v>70</v>
@@ -41452,7 +41449,7 @@
         <v>81</v>
       </c>
       <c r="U45" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V45" s="160" t="s">
         <v>70</v>
@@ -42513,7 +42510,7 @@
         <v>81</v>
       </c>
       <c r="U46" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V46" s="160" t="s">
         <v>70</v>
@@ -43574,7 +43571,7 @@
         <v>81</v>
       </c>
       <c r="U47" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V47" s="160" t="s">
         <v>70</v>
@@ -44635,7 +44632,7 @@
         <v>81</v>
       </c>
       <c r="U48" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V48" s="160" t="s">
         <v>70</v>
@@ -45696,7 +45693,7 @@
         <v>81</v>
       </c>
       <c r="U49" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V49" s="160" t="s">
         <v>70</v>
@@ -46758,7 +46755,7 @@
       </c>
       <c r="T50"/>
       <c r="U50" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V50" s="160" t="s">
         <v>70</v>
@@ -46829,7 +46826,7 @@
         <v>81</v>
       </c>
       <c r="U51" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V51" s="160" t="s">
         <v>70</v>
@@ -47890,7 +47887,7 @@
         <v>81</v>
       </c>
       <c r="U52" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V52" s="160" t="s">
         <v>70</v>
@@ -48951,7 +48948,7 @@
         <v>81</v>
       </c>
       <c r="U53" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V53" s="160" t="s">
         <v>70</v>
@@ -50012,7 +50009,7 @@
         <v>81</v>
       </c>
       <c r="U54" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V54" s="160" t="s">
         <v>70</v>
@@ -51073,7 +51070,7 @@
         <v>81</v>
       </c>
       <c r="U55" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V55" s="160" t="s">
         <v>70</v>
@@ -52134,7 +52131,7 @@
         <v>81</v>
       </c>
       <c r="U56" s="159" t="s">
-        <v>840</v>
+        <v>165</v>
       </c>
       <c r="V56" s="160" t="s">
         <v>70</v>

</xml_diff>